<commit_message>
columns of the primary types are now cast into those types to ensure data integrity on a per-column basis
</commit_message>
<xml_diff>
--- a/tmp_sheets/MIGRATION_Items_Markup.xlsx
+++ b/tmp_sheets/MIGRATION_Items_Markup.xlsx
@@ -576,7 +576,11 @@
           <t>Club</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="D3" t="n">
         <v>5</v>
       </c>
@@ -599,18 +603,18 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L3" t="b">
+        <v>1</v>
+      </c>
+      <c r="M3" t="b">
+        <v>1</v>
+      </c>
       <c r="N3" t="n">
         <v>-1</v>
       </c>
@@ -626,8 +630,12 @@
           <t>Dagger</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="b">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
@@ -649,18 +657,18 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L4" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4" t="b">
+        <v>1</v>
+      </c>
       <c r="N4" t="n">
         <v>-1</v>
       </c>
@@ -676,7 +684,11 @@
           <t>Spear / Pike / Halberd</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="D5" t="n">
         <v>2</v>
       </c>
@@ -699,18 +711,18 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M5" t="b">
+        <v>1</v>
+      </c>
       <c r="N5" t="n">
         <v>-1</v>
       </c>
@@ -726,8 +738,12 @@
           <t>Shortsword</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="b">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
         <v>1</v>
       </c>
       <c r="E6" t="n">
@@ -749,18 +765,18 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6" t="b">
+        <v>1</v>
+      </c>
+      <c r="M6" t="b">
+        <v>1</v>
+      </c>
       <c r="N6" t="n">
         <v>-1</v>
       </c>
@@ -776,8 +792,12 @@
           <t>Longsword</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="b">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
         <v>1</v>
       </c>
       <c r="E7" t="n">
@@ -799,18 +819,18 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
+      <c r="J7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" t="b">
+        <v>1</v>
+      </c>
+      <c r="L7" t="b">
+        <v>1</v>
+      </c>
+      <c r="M7" t="b">
+        <v>1</v>
+      </c>
       <c r="N7" t="n">
         <v>-1</v>
       </c>
@@ -826,8 +846,12 @@
           <t>Great Sword (2H)</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="b">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
         <v>1</v>
       </c>
       <c r="E8" t="n">
@@ -849,18 +873,18 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" t="b">
+        <v>1</v>
+      </c>
+      <c r="L8" t="b">
+        <v>1</v>
+      </c>
+      <c r="M8" t="b">
+        <v>1</v>
+      </c>
       <c r="N8" t="n">
         <v>-1</v>
       </c>
@@ -876,7 +900,11 @@
           <t>Sling (x1)</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="D9" t="n">
         <v>5</v>
       </c>
@@ -899,18 +927,18 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
+      <c r="J9" t="b">
+        <v>1</v>
+      </c>
+      <c r="K9" t="b">
+        <v>1</v>
+      </c>
+      <c r="L9" t="b">
+        <v>1</v>
+      </c>
+      <c r="M9" t="b">
+        <v>1</v>
+      </c>
       <c r="N9" t="n">
         <v>-1</v>
       </c>
@@ -926,7 +954,11 @@
           <t>Buckler</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
@@ -949,17 +981,17 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" t="b">
+        <v>1</v>
+      </c>
+      <c r="L10" t="b">
+        <v>1</v>
+      </c>
+      <c r="M10" t="b">
+        <v>1</v>
       </c>
       <c r="N10" t="n">
         <v>-1</v>
@@ -976,7 +1008,11 @@
           <t>Heavy Cloth Armor</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
@@ -999,18 +1035,18 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr"/>
+      <c r="J11" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" t="b">
+        <v>1</v>
+      </c>
+      <c r="L11" t="b">
+        <v>1</v>
+      </c>
+      <c r="M11" t="b">
+        <v>1</v>
+      </c>
       <c r="N11" t="n">
         <v>-1</v>
       </c>
@@ -1026,7 +1062,11 @@
           <t>Leather Armor</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="D12" t="n">
         <v>0</v>
       </c>
@@ -1049,18 +1089,18 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr"/>
+      <c r="J12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" t="b">
+        <v>1</v>
+      </c>
+      <c r="L12" t="b">
+        <v>1</v>
+      </c>
+      <c r="M12" t="b">
+        <v>1</v>
+      </c>
       <c r="N12" t="n">
         <v>-1</v>
       </c>
@@ -1103,14 +1143,18 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
+      <c r="J13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K13" t="b">
+        <v>1</v>
+      </c>
+      <c r="L13" t="b">
+        <v>1</v>
+      </c>
+      <c r="M13" t="b">
+        <v>1</v>
+      </c>
       <c r="N13" t="n">
         <v>-1</v>
       </c>
@@ -1126,7 +1170,11 @@
           <t>Studded Leather Armor</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="D14" t="n">
         <v>0</v>
       </c>
@@ -1149,18 +1197,18 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr"/>
+      <c r="J14" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" t="b">
+        <v>1</v>
+      </c>
+      <c r="L14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M14" t="b">
+        <v>1</v>
+      </c>
       <c r="N14" t="n">
         <v>-1</v>
       </c>
@@ -1176,7 +1224,11 @@
           <t>Chain Mail</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="D15" t="n">
         <v>0</v>
       </c>
@@ -1199,18 +1251,18 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr"/>
+      <c r="J15" t="b">
+        <v>1</v>
+      </c>
+      <c r="K15" t="b">
+        <v>1</v>
+      </c>
+      <c r="L15" t="b">
+        <v>1</v>
+      </c>
+      <c r="M15" t="b">
+        <v>1</v>
+      </c>
       <c r="N15" t="n">
         <v>-1</v>
       </c>
@@ -1226,7 +1278,11 @@
           <t>Plate Mail</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr"/>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="D16" t="n">
         <v>0</v>
       </c>
@@ -1249,18 +1305,18 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr"/>
+      <c r="J16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K16" t="b">
+        <v>1</v>
+      </c>
+      <c r="L16" t="b">
+        <v>1</v>
+      </c>
+      <c r="M16" t="b">
+        <v>1</v>
+      </c>
       <c r="N16" t="n">
         <v>-1</v>
       </c>
@@ -1276,8 +1332,12 @@
           <t>Warhammer (2H)</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="b">
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
         <v>1</v>
       </c>
       <c r="E17" t="n">
@@ -1299,18 +1359,18 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr"/>
+      <c r="J17" t="b">
+        <v>1</v>
+      </c>
+      <c r="K17" t="b">
+        <v>1</v>
+      </c>
+      <c r="L17" t="b">
+        <v>1</v>
+      </c>
+      <c r="M17" t="b">
+        <v>1</v>
+      </c>
       <c r="N17" t="n">
         <v>-1</v>
       </c>
@@ -1326,8 +1386,12 @@
           <t>Battle Axe</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="b">
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
         <v>1</v>
       </c>
       <c r="E18" t="n">
@@ -1349,18 +1413,18 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="L18" t="inlineStr"/>
-      <c r="M18" t="inlineStr"/>
+      <c r="J18" t="b">
+        <v>1</v>
+      </c>
+      <c r="K18" t="b">
+        <v>1</v>
+      </c>
+      <c r="L18" t="b">
+        <v>1</v>
+      </c>
+      <c r="M18" t="b">
+        <v>1</v>
+      </c>
       <c r="N18" t="n">
         <v>-1</v>
       </c>
@@ -1376,8 +1440,12 @@
           <t>Wizards Staff (2H)</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="b">
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
         <v>1</v>
       </c>
       <c r="E19" t="n">
@@ -1399,18 +1467,18 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="L19" t="inlineStr"/>
-      <c r="M19" t="inlineStr"/>
+      <c r="J19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K19" t="b">
+        <v>1</v>
+      </c>
+      <c r="L19" t="b">
+        <v>1</v>
+      </c>
+      <c r="M19" t="b">
+        <v>1</v>
+      </c>
       <c r="N19" t="n">
         <v>-1</v>
       </c>
@@ -1453,18 +1521,18 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="L20" t="inlineStr"/>
-      <c r="M20" t="inlineStr"/>
+      <c r="J20" t="b">
+        <v>1</v>
+      </c>
+      <c r="K20" t="b">
+        <v>1</v>
+      </c>
+      <c r="L20" t="b">
+        <v>1</v>
+      </c>
+      <c r="M20" t="b">
+        <v>1</v>
+      </c>
       <c r="N20" t="n">
         <v>-1</v>
       </c>
@@ -1507,18 +1575,18 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="L21" t="inlineStr"/>
-      <c r="M21" t="inlineStr"/>
+      <c r="J21" t="b">
+        <v>1</v>
+      </c>
+      <c r="K21" t="b">
+        <v>1</v>
+      </c>
+      <c r="L21" t="b">
+        <v>1</v>
+      </c>
+      <c r="M21" t="b">
+        <v>1</v>
+      </c>
       <c r="N21" t="n">
         <v>-1</v>
       </c>
@@ -1561,18 +1629,18 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="L22" t="inlineStr"/>
-      <c r="M22" t="inlineStr"/>
+      <c r="J22" t="b">
+        <v>1</v>
+      </c>
+      <c r="K22" t="b">
+        <v>1</v>
+      </c>
+      <c r="L22" t="b">
+        <v>1</v>
+      </c>
+      <c r="M22" t="b">
+        <v>1</v>
+      </c>
       <c r="N22" t="n">
         <v>-1</v>
       </c>
@@ -1615,18 +1683,18 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="L23" t="inlineStr"/>
-      <c r="M23" t="inlineStr"/>
+      <c r="J23" t="b">
+        <v>1</v>
+      </c>
+      <c r="K23" t="b">
+        <v>1</v>
+      </c>
+      <c r="L23" t="b">
+        <v>1</v>
+      </c>
+      <c r="M23" t="b">
+        <v>1</v>
+      </c>
       <c r="N23" t="n">
         <v>-1</v>
       </c>
@@ -1669,18 +1737,18 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="L24" t="inlineStr"/>
-      <c r="M24" t="inlineStr"/>
+      <c r="J24" t="b">
+        <v>1</v>
+      </c>
+      <c r="K24" t="b">
+        <v>1</v>
+      </c>
+      <c r="L24" t="b">
+        <v>1</v>
+      </c>
+      <c r="M24" t="b">
+        <v>1</v>
+      </c>
       <c r="N24" t="n">
         <v>-1</v>
       </c>
@@ -1723,18 +1791,18 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="L25" t="inlineStr"/>
-      <c r="M25" t="inlineStr"/>
+      <c r="J25" t="b">
+        <v>1</v>
+      </c>
+      <c r="K25" t="b">
+        <v>1</v>
+      </c>
+      <c r="L25" t="b">
+        <v>1</v>
+      </c>
+      <c r="M25" t="b">
+        <v>1</v>
+      </c>
       <c r="N25" t="n">
         <v>-1</v>
       </c>
@@ -1750,7 +1818,11 @@
           <t>Kite Shield</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr"/>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="n">
         <v>0</v>
@@ -1771,17 +1843,17 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr"/>
-      <c r="L26" t="inlineStr"/>
-      <c r="M26" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
+      <c r="J26" t="b">
+        <v>1</v>
+      </c>
+      <c r="K26" t="b">
+        <v>1</v>
+      </c>
+      <c r="L26" t="b">
+        <v>1</v>
+      </c>
+      <c r="M26" t="b">
+        <v>1</v>
       </c>
       <c r="N26" t="n">
         <v>-1</v>
@@ -1819,14 +1891,18 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K27" t="inlineStr"/>
-      <c r="L27" t="inlineStr"/>
-      <c r="M27" t="inlineStr"/>
+      <c r="J27" t="b">
+        <v>1</v>
+      </c>
+      <c r="K27" t="b">
+        <v>1</v>
+      </c>
+      <c r="L27" t="b">
+        <v>1</v>
+      </c>
+      <c r="M27" t="b">
+        <v>1</v>
+      </c>
       <c r="N27" t="n">
         <v>-1</v>
       </c>
@@ -1863,14 +1939,18 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr"/>
-      <c r="L28" t="inlineStr"/>
-      <c r="M28" t="inlineStr"/>
+      <c r="J28" t="b">
+        <v>1</v>
+      </c>
+      <c r="K28" t="b">
+        <v>1</v>
+      </c>
+      <c r="L28" t="b">
+        <v>1</v>
+      </c>
+      <c r="M28" t="b">
+        <v>1</v>
+      </c>
       <c r="N28" t="n">
         <v>-1</v>
       </c>
@@ -1909,14 +1989,18 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr"/>
-      <c r="L29" t="inlineStr"/>
-      <c r="M29" t="inlineStr"/>
+      <c r="J29" t="b">
+        <v>1</v>
+      </c>
+      <c r="K29" t="b">
+        <v>1</v>
+      </c>
+      <c r="L29" t="b">
+        <v>1</v>
+      </c>
+      <c r="M29" t="b">
+        <v>1</v>
+      </c>
       <c r="N29" t="n">
         <v>-1</v>
       </c>
@@ -1937,7 +2021,7 @@
           <t>During a scene, restore 2D6 Hitpoints Points to yourself when not adjacent to an enemy using an Interact action. 1 Charge.</t>
         </is>
       </c>
-      <c r="D30" t="b">
+      <c r="D30" t="n">
         <v>1</v>
       </c>
       <c r="E30" t="inlineStr"/>
@@ -1955,14 +2039,18 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K30" t="inlineStr"/>
-      <c r="L30" t="inlineStr"/>
-      <c r="M30" t="inlineStr"/>
+      <c r="J30" t="b">
+        <v>1</v>
+      </c>
+      <c r="K30" t="b">
+        <v>1</v>
+      </c>
+      <c r="L30" t="b">
+        <v>1</v>
+      </c>
+      <c r="M30" t="b">
+        <v>1</v>
+      </c>
       <c r="N30" t="n">
         <v>-1</v>
       </c>
@@ -2000,14 +2088,18 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K31" t="inlineStr"/>
-      <c r="L31" t="inlineStr"/>
-      <c r="M31" t="inlineStr"/>
+      <c r="J31" t="b">
+        <v>1</v>
+      </c>
+      <c r="K31" t="b">
+        <v>1</v>
+      </c>
+      <c r="L31" t="b">
+        <v>1</v>
+      </c>
+      <c r="M31" t="b">
+        <v>1</v>
+      </c>
       <c r="N31" t="n">
         <v>-1</v>
       </c>
@@ -2044,14 +2136,18 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K32" t="inlineStr"/>
-      <c r="L32" t="inlineStr"/>
-      <c r="M32" t="inlineStr"/>
+      <c r="J32" t="b">
+        <v>1</v>
+      </c>
+      <c r="K32" t="b">
+        <v>1</v>
+      </c>
+      <c r="L32" t="b">
+        <v>1</v>
+      </c>
+      <c r="M32" t="b">
+        <v>1</v>
+      </c>
       <c r="N32" t="n">
         <v>-1</v>
       </c>
@@ -2088,14 +2184,18 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K33" t="inlineStr"/>
-      <c r="L33" t="inlineStr"/>
-      <c r="M33" t="inlineStr"/>
+      <c r="J33" t="b">
+        <v>1</v>
+      </c>
+      <c r="K33" t="b">
+        <v>1</v>
+      </c>
+      <c r="L33" t="b">
+        <v>1</v>
+      </c>
+      <c r="M33" t="b">
+        <v>1</v>
+      </c>
       <c r="N33" t="n">
         <v>-1</v>
       </c>
@@ -2132,14 +2232,18 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K34" t="inlineStr"/>
-      <c r="L34" t="inlineStr"/>
-      <c r="M34" t="inlineStr"/>
+      <c r="J34" t="b">
+        <v>1</v>
+      </c>
+      <c r="K34" t="b">
+        <v>1</v>
+      </c>
+      <c r="L34" t="b">
+        <v>1</v>
+      </c>
+      <c r="M34" t="b">
+        <v>1</v>
+      </c>
       <c r="N34" t="n">
         <v>-1</v>
       </c>
@@ -2176,14 +2280,18 @@
           <t>Medieval</t>
         </is>
       </c>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K35" t="inlineStr"/>
-      <c r="L35" t="inlineStr"/>
-      <c r="M35" t="inlineStr"/>
+      <c r="J35" t="b">
+        <v>1</v>
+      </c>
+      <c r="K35" t="b">
+        <v>1</v>
+      </c>
+      <c r="L35" t="b">
+        <v>1</v>
+      </c>
+      <c r="M35" t="b">
+        <v>1</v>
+      </c>
       <c r="N35" t="n">
         <v>-1</v>
       </c>

</xml_diff>

<commit_message>
fix "nan" in blank text cells bug format datetime columns and convert them to strings
</commit_message>
<xml_diff>
--- a/tmp_sheets/MIGRATION_Items_Markup.xlsx
+++ b/tmp_sheets/MIGRATION_Items_Markup.xlsx
@@ -576,11 +576,7 @@
           <t>Club</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
         <v>5</v>
       </c>
@@ -609,12 +605,8 @@
       <c r="K3" t="b">
         <v>1</v>
       </c>
-      <c r="L3" t="b">
-        <v>1</v>
-      </c>
-      <c r="M3" t="b">
-        <v>1</v>
-      </c>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
       <c r="N3" t="n">
         <v>-1</v>
       </c>
@@ -630,11 +622,7 @@
           <t>Dagger</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
         <v>1</v>
       </c>
@@ -663,12 +651,8 @@
       <c r="K4" t="b">
         <v>1</v>
       </c>
-      <c r="L4" t="b">
-        <v>1</v>
-      </c>
-      <c r="M4" t="b">
-        <v>1</v>
-      </c>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
       <c r="N4" t="n">
         <v>-1</v>
       </c>
@@ -684,11 +668,7 @@
           <t>Spear / Pike / Halberd</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
         <v>2</v>
       </c>
@@ -717,12 +697,8 @@
       <c r="K5" t="b">
         <v>1</v>
       </c>
-      <c r="L5" t="b">
-        <v>1</v>
-      </c>
-      <c r="M5" t="b">
-        <v>1</v>
-      </c>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
       <c r="N5" t="n">
         <v>-1</v>
       </c>
@@ -738,11 +714,7 @@
           <t>Shortsword</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
         <v>1</v>
       </c>
@@ -771,12 +743,8 @@
       <c r="K6" t="b">
         <v>1</v>
       </c>
-      <c r="L6" t="b">
-        <v>1</v>
-      </c>
-      <c r="M6" t="b">
-        <v>1</v>
-      </c>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
       <c r="N6" t="n">
         <v>-1</v>
       </c>
@@ -792,11 +760,7 @@
           <t>Longsword</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
         <v>1</v>
       </c>
@@ -825,12 +789,8 @@
       <c r="K7" t="b">
         <v>1</v>
       </c>
-      <c r="L7" t="b">
-        <v>1</v>
-      </c>
-      <c r="M7" t="b">
-        <v>1</v>
-      </c>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
       <c r="N7" t="n">
         <v>-1</v>
       </c>
@@ -846,11 +806,7 @@
           <t>Great Sword (2H)</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
         <v>1</v>
       </c>
@@ -879,12 +835,8 @@
       <c r="K8" t="b">
         <v>1</v>
       </c>
-      <c r="L8" t="b">
-        <v>1</v>
-      </c>
-      <c r="M8" t="b">
-        <v>1</v>
-      </c>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
       <c r="N8" t="n">
         <v>-1</v>
       </c>
@@ -900,11 +852,7 @@
           <t>Sling (x1)</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="C9" t="inlineStr"/>
       <c r="D9" t="n">
         <v>5</v>
       </c>
@@ -933,12 +881,8 @@
       <c r="K9" t="b">
         <v>1</v>
       </c>
-      <c r="L9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M9" t="b">
-        <v>1</v>
-      </c>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
       <c r="N9" t="n">
         <v>-1</v>
       </c>
@@ -954,11 +898,7 @@
           <t>Buckler</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
         <v>0</v>
       </c>
@@ -984,12 +924,8 @@
       <c r="J10" t="b">
         <v>1</v>
       </c>
-      <c r="K10" t="b">
-        <v>1</v>
-      </c>
-      <c r="L10" t="b">
-        <v>1</v>
-      </c>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
       <c r="M10" t="b">
         <v>1</v>
       </c>
@@ -1008,11 +944,7 @@
           <t>Heavy Cloth Armor</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="C11" t="inlineStr"/>
       <c r="D11" t="n">
         <v>0</v>
       </c>
@@ -1038,15 +970,11 @@
       <c r="J11" t="b">
         <v>1</v>
       </c>
-      <c r="K11" t="b">
-        <v>1</v>
-      </c>
+      <c r="K11" t="inlineStr"/>
       <c r="L11" t="b">
         <v>1</v>
       </c>
-      <c r="M11" t="b">
-        <v>1</v>
-      </c>
+      <c r="M11" t="inlineStr"/>
       <c r="N11" t="n">
         <v>-1</v>
       </c>
@@ -1062,11 +990,7 @@
           <t>Leather Armor</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="C12" t="inlineStr"/>
       <c r="D12" t="n">
         <v>0</v>
       </c>
@@ -1092,15 +1016,11 @@
       <c r="J12" t="b">
         <v>1</v>
       </c>
-      <c r="K12" t="b">
-        <v>1</v>
-      </c>
+      <c r="K12" t="inlineStr"/>
       <c r="L12" t="b">
         <v>1</v>
       </c>
-      <c r="M12" t="b">
-        <v>1</v>
-      </c>
+      <c r="M12" t="inlineStr"/>
       <c r="N12" t="n">
         <v>-1</v>
       </c>
@@ -1146,15 +1066,9 @@
       <c r="J13" t="b">
         <v>1</v>
       </c>
-      <c r="K13" t="b">
-        <v>1</v>
-      </c>
-      <c r="L13" t="b">
-        <v>1</v>
-      </c>
-      <c r="M13" t="b">
-        <v>1</v>
-      </c>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
       <c r="N13" t="n">
         <v>-1</v>
       </c>
@@ -1170,11 +1084,7 @@
           <t>Studded Leather Armor</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="C14" t="inlineStr"/>
       <c r="D14" t="n">
         <v>0</v>
       </c>
@@ -1200,15 +1110,11 @@
       <c r="J14" t="b">
         <v>1</v>
       </c>
-      <c r="K14" t="b">
-        <v>1</v>
-      </c>
+      <c r="K14" t="inlineStr"/>
       <c r="L14" t="b">
         <v>1</v>
       </c>
-      <c r="M14" t="b">
-        <v>1</v>
-      </c>
+      <c r="M14" t="inlineStr"/>
       <c r="N14" t="n">
         <v>-1</v>
       </c>
@@ -1224,11 +1130,7 @@
           <t>Chain Mail</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="C15" t="inlineStr"/>
       <c r="D15" t="n">
         <v>0</v>
       </c>
@@ -1254,15 +1156,11 @@
       <c r="J15" t="b">
         <v>1</v>
       </c>
-      <c r="K15" t="b">
-        <v>1</v>
-      </c>
+      <c r="K15" t="inlineStr"/>
       <c r="L15" t="b">
         <v>1</v>
       </c>
-      <c r="M15" t="b">
-        <v>1</v>
-      </c>
+      <c r="M15" t="inlineStr"/>
       <c r="N15" t="n">
         <v>-1</v>
       </c>
@@ -1278,11 +1176,7 @@
           <t>Plate Mail</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="C16" t="inlineStr"/>
       <c r="D16" t="n">
         <v>0</v>
       </c>
@@ -1308,15 +1202,11 @@
       <c r="J16" t="b">
         <v>1</v>
       </c>
-      <c r="K16" t="b">
-        <v>1</v>
-      </c>
+      <c r="K16" t="inlineStr"/>
       <c r="L16" t="b">
         <v>1</v>
       </c>
-      <c r="M16" t="b">
-        <v>1</v>
-      </c>
+      <c r="M16" t="inlineStr"/>
       <c r="N16" t="n">
         <v>-1</v>
       </c>
@@ -1332,11 +1222,7 @@
           <t>Warhammer (2H)</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="C17" t="inlineStr"/>
       <c r="D17" t="n">
         <v>1</v>
       </c>
@@ -1365,12 +1251,8 @@
       <c r="K17" t="b">
         <v>1</v>
       </c>
-      <c r="L17" t="b">
-        <v>1</v>
-      </c>
-      <c r="M17" t="b">
-        <v>1</v>
-      </c>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
       <c r="N17" t="n">
         <v>-1</v>
       </c>
@@ -1386,11 +1268,7 @@
           <t>Battle Axe</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="C18" t="inlineStr"/>
       <c r="D18" t="n">
         <v>1</v>
       </c>
@@ -1419,12 +1297,8 @@
       <c r="K18" t="b">
         <v>1</v>
       </c>
-      <c r="L18" t="b">
-        <v>1</v>
-      </c>
-      <c r="M18" t="b">
-        <v>1</v>
-      </c>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
       <c r="N18" t="n">
         <v>-1</v>
       </c>
@@ -1440,11 +1314,7 @@
           <t>Wizards Staff (2H)</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="C19" t="inlineStr"/>
       <c r="D19" t="n">
         <v>1</v>
       </c>
@@ -1473,12 +1343,8 @@
       <c r="K19" t="b">
         <v>1</v>
       </c>
-      <c r="L19" t="b">
-        <v>1</v>
-      </c>
-      <c r="M19" t="b">
-        <v>1</v>
-      </c>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
       <c r="N19" t="n">
         <v>-1</v>
       </c>
@@ -1527,12 +1393,8 @@
       <c r="K20" t="b">
         <v>1</v>
       </c>
-      <c r="L20" t="b">
-        <v>1</v>
-      </c>
-      <c r="M20" t="b">
-        <v>1</v>
-      </c>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
       <c r="N20" t="n">
         <v>-1</v>
       </c>
@@ -1581,12 +1443,8 @@
       <c r="K21" t="b">
         <v>1</v>
       </c>
-      <c r="L21" t="b">
-        <v>1</v>
-      </c>
-      <c r="M21" t="b">
-        <v>1</v>
-      </c>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
       <c r="N21" t="n">
         <v>-1</v>
       </c>
@@ -1635,12 +1493,8 @@
       <c r="K22" t="b">
         <v>1</v>
       </c>
-      <c r="L22" t="b">
-        <v>1</v>
-      </c>
-      <c r="M22" t="b">
-        <v>1</v>
-      </c>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
       <c r="N22" t="n">
         <v>-1</v>
       </c>
@@ -1689,12 +1543,8 @@
       <c r="K23" t="b">
         <v>1</v>
       </c>
-      <c r="L23" t="b">
-        <v>1</v>
-      </c>
-      <c r="M23" t="b">
-        <v>1</v>
-      </c>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
       <c r="N23" t="n">
         <v>-1</v>
       </c>
@@ -1743,12 +1593,8 @@
       <c r="K24" t="b">
         <v>1</v>
       </c>
-      <c r="L24" t="b">
-        <v>1</v>
-      </c>
-      <c r="M24" t="b">
-        <v>1</v>
-      </c>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
       <c r="N24" t="n">
         <v>-1</v>
       </c>
@@ -1797,12 +1643,8 @@
       <c r="K25" t="b">
         <v>1</v>
       </c>
-      <c r="L25" t="b">
-        <v>1</v>
-      </c>
-      <c r="M25" t="b">
-        <v>1</v>
-      </c>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
       <c r="N25" t="n">
         <v>-1</v>
       </c>
@@ -1818,11 +1660,7 @@
           <t>Kite Shield</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="n">
         <v>0</v>
@@ -1846,12 +1684,8 @@
       <c r="J26" t="b">
         <v>1</v>
       </c>
-      <c r="K26" t="b">
-        <v>1</v>
-      </c>
-      <c r="L26" t="b">
-        <v>1</v>
-      </c>
+      <c r="K26" t="inlineStr"/>
+      <c r="L26" t="inlineStr"/>
       <c r="M26" t="b">
         <v>1</v>
       </c>
@@ -1894,15 +1728,9 @@
       <c r="J27" t="b">
         <v>1</v>
       </c>
-      <c r="K27" t="b">
-        <v>1</v>
-      </c>
-      <c r="L27" t="b">
-        <v>1</v>
-      </c>
-      <c r="M27" t="b">
-        <v>1</v>
-      </c>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
       <c r="N27" t="n">
         <v>-1</v>
       </c>
@@ -1942,15 +1770,9 @@
       <c r="J28" t="b">
         <v>1</v>
       </c>
-      <c r="K28" t="b">
-        <v>1</v>
-      </c>
-      <c r="L28" t="b">
-        <v>1</v>
-      </c>
-      <c r="M28" t="b">
-        <v>1</v>
-      </c>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
       <c r="N28" t="n">
         <v>-1</v>
       </c>
@@ -1992,15 +1814,9 @@
       <c r="J29" t="b">
         <v>1</v>
       </c>
-      <c r="K29" t="b">
-        <v>1</v>
-      </c>
-      <c r="L29" t="b">
-        <v>1</v>
-      </c>
-      <c r="M29" t="b">
-        <v>1</v>
-      </c>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
       <c r="N29" t="n">
         <v>-1</v>
       </c>
@@ -2042,15 +1858,9 @@
       <c r="J30" t="b">
         <v>1</v>
       </c>
-      <c r="K30" t="b">
-        <v>1</v>
-      </c>
-      <c r="L30" t="b">
-        <v>1</v>
-      </c>
-      <c r="M30" t="b">
-        <v>1</v>
-      </c>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr"/>
       <c r="N30" t="n">
         <v>-1</v>
       </c>
@@ -2091,15 +1901,9 @@
       <c r="J31" t="b">
         <v>1</v>
       </c>
-      <c r="K31" t="b">
-        <v>1</v>
-      </c>
-      <c r="L31" t="b">
-        <v>1</v>
-      </c>
-      <c r="M31" t="b">
-        <v>1</v>
-      </c>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr"/>
+      <c r="M31" t="inlineStr"/>
       <c r="N31" t="n">
         <v>-1</v>
       </c>
@@ -2139,15 +1943,9 @@
       <c r="J32" t="b">
         <v>1</v>
       </c>
-      <c r="K32" t="b">
-        <v>1</v>
-      </c>
-      <c r="L32" t="b">
-        <v>1</v>
-      </c>
-      <c r="M32" t="b">
-        <v>1</v>
-      </c>
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
       <c r="N32" t="n">
         <v>-1</v>
       </c>
@@ -2187,15 +1985,9 @@
       <c r="J33" t="b">
         <v>1</v>
       </c>
-      <c r="K33" t="b">
-        <v>1</v>
-      </c>
-      <c r="L33" t="b">
-        <v>1</v>
-      </c>
-      <c r="M33" t="b">
-        <v>1</v>
-      </c>
+      <c r="K33" t="inlineStr"/>
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="inlineStr"/>
       <c r="N33" t="n">
         <v>-1</v>
       </c>
@@ -2235,15 +2027,9 @@
       <c r="J34" t="b">
         <v>1</v>
       </c>
-      <c r="K34" t="b">
-        <v>1</v>
-      </c>
-      <c r="L34" t="b">
-        <v>1</v>
-      </c>
-      <c r="M34" t="b">
-        <v>1</v>
-      </c>
+      <c r="K34" t="inlineStr"/>
+      <c r="L34" t="inlineStr"/>
+      <c r="M34" t="inlineStr"/>
       <c r="N34" t="n">
         <v>-1</v>
       </c>
@@ -2283,15 +2069,9 @@
       <c r="J35" t="b">
         <v>1</v>
       </c>
-      <c r="K35" t="b">
-        <v>1</v>
-      </c>
-      <c r="L35" t="b">
-        <v>1</v>
-      </c>
-      <c r="M35" t="b">
-        <v>1</v>
-      </c>
+      <c r="K35" t="inlineStr"/>
+      <c r="L35" t="inlineStr"/>
+      <c r="M35" t="inlineStr"/>
       <c r="N35" t="n">
         <v>-1</v>
       </c>

</xml_diff>